<commit_message>
load 4 domain and group by ip
</commit_message>
<xml_diff>
--- a/data/Book1.xlsx
+++ b/data/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dragonfly/Documents/scan_ip/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBA3414-E0E8-D240-BFD1-F97698009DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCC5718-3C4C-9547-868A-4EE109EBA323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{0E922DF3-AA5B-4714-95F4-706A488422E4}"/>
   </bookViews>
@@ -256,10 +256,10 @@
     <t>tiktok.com</t>
   </si>
   <si>
-    <t>quora.com</t>
-  </si>
-  <si>
     <t>bing.com</t>
+  </si>
+  <si>
+    <t>x.com</t>
   </si>
 </sst>
 </file>
@@ -897,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{541B1F19-64BE-4561-8C74-74087608BBB1}">
   <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="174" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="174" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1039,7 +1039,7 @@
         <v>62</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V2" s="12"/>
     </row>
@@ -1137,7 +1137,7 @@
         <v>64</v>
       </c>
       <c r="U4" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="V4" s="12"/>
     </row>

</xml_diff>

<commit_message>
use whois for check subnet
</commit_message>
<xml_diff>
--- a/data/Book1.xlsx
+++ b/data/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dragonfly/Documents/scan_ip/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCC5718-3C4C-9547-868A-4EE109EBA323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CC27B7-7223-2A44-8058-DE41DA4AE97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{0E922DF3-AA5B-4714-95F4-706A488422E4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
   <si>
     <t>PHẦN NÀY LẤY NGUYÊN TỪ DANH SÁCH APP ID DO TTPT PM GỬI</t>
   </si>
@@ -239,9 +239,6 @@
   </si>
   <si>
     <t>youtube.com</t>
-  </si>
-  <si>
-    <t>24h.vn</t>
   </si>
   <si>
     <t>apple.com</t>
@@ -897,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{541B1F19-64BE-4561-8C74-74087608BBB1}">
   <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="174" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="174" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1036,10 +1033,10 @@
         <v>59</v>
       </c>
       <c r="T2" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="V2" s="12"/>
     </row>
@@ -1079,10 +1076,10 @@
         <v>56</v>
       </c>
       <c r="S3" s="14" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="T3" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U3" s="14" t="s">
         <v>58</v>
@@ -1131,13 +1128,13 @@
         <v>57</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="T4" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="U4" s="12" t="s">
         <v>64</v>
-      </c>
-      <c r="U4" s="12" t="s">
-        <v>65</v>
       </c>
       <c r="V4" s="12"/>
     </row>

</xml_diff>

<commit_message>
edit all file main and add check empty domain
</commit_message>
<xml_diff>
--- a/data/Book1.xlsx
+++ b/data/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dragonfly/Documents/scan_ip/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CC27B7-7223-2A44-8058-DE41DA4AE97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{536BA915-6373-BC47-9C63-E997333CEA6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{0E922DF3-AA5B-4714-95F4-706A488422E4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
   <si>
     <t>PHẦN NÀY LẤY NGUYÊN TỪ DANH SÁCH APP ID DO TTPT PM GỬI</t>
   </si>
@@ -238,15 +238,9 @@
     <t>github.com</t>
   </si>
   <si>
-    <t>youtube.com</t>
-  </si>
-  <si>
     <t>apple.com</t>
   </si>
   <si>
-    <t>wikipedia.com</t>
-  </si>
-  <si>
     <t>shopee.vn</t>
   </si>
   <si>
@@ -256,7 +250,7 @@
     <t>bing.com</t>
   </si>
   <si>
-    <t>x.com</t>
+    <t>dsfdfds.sdgdg</t>
   </si>
 </sst>
 </file>
@@ -894,8 +888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{541B1F19-64BE-4561-8C74-74087608BBB1}">
   <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="174" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="174" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1030,13 +1024,13 @@
         <v>55</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="T2" s="12" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="V2" s="12"/>
     </row>
@@ -1076,10 +1070,10 @@
         <v>56</v>
       </c>
       <c r="S3" s="14" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="T3" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="U3" s="14" t="s">
         <v>58</v>
@@ -1128,13 +1122,13 @@
         <v>57</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="U4" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="V4" s="12"/>
     </row>

</xml_diff>